<commit_message>
Grosse modif ! Automatisation terminée Nouveaux graphiques
</commit_message>
<xml_diff>
--- a/99__Documents/Data_synthese.xlsx
+++ b/99__Documents/Data_synthese.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="172">
   <si>
     <t>Synthese TRAIN</t>
   </si>
@@ -145,6 +145,15 @@
     <t>34</t>
   </si>
   <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -247,6 +256,15 @@
     <t>prime_tot_ttc</t>
   </si>
   <si>
+    <t>prix_ref</t>
+  </si>
+  <si>
+    <t>AD_val</t>
+  </si>
+  <si>
+    <t>count_AD_val</t>
+  </si>
+  <si>
     <t>integer</t>
   </si>
   <si>
@@ -262,15 +280,6 @@
     <t>0.10%</t>
   </si>
   <si>
-    <t>0.14%</t>
-  </si>
-  <si>
-    <t>0.20%</t>
-  </si>
-  <si>
-    <t>0.11%</t>
-  </si>
-  <si>
     <t>1/2/3/4/5/6</t>
   </si>
   <si>
@@ -292,7 +301,7 @@
     <t>1034/1001/1002/1004/1005/1007</t>
   </si>
   <si>
-    <t>gpl/hybride essence/electricite/gazole/essence</t>
+    <t>gpl/hybride essence/electricite/gazole/essence/NR</t>
   </si>
   <si>
     <t>2924/11580/7149/6526/2872/7191</t>
@@ -367,6 +376,12 @@
     <t>254.75/259.89/431.65/577.99/222.67/595.23</t>
   </si>
   <si>
+    <t>374.632352941176/519.78/454.368421052632/577.99/445.34/595.23</t>
+  </si>
+  <si>
+    <t>0.47/0/0.01/0.02/0.07/0.03</t>
+  </si>
+  <si>
     <t>Synthese TEST</t>
   </si>
   <si>
@@ -379,6 +394,9 @@
     <t>0.06%</t>
   </si>
   <si>
+    <t>97109/97110/97111/97112/97113/97114</t>
+  </si>
+  <si>
     <t>2/36/3/1/0/33</t>
   </si>
   <si>
@@ -388,13 +406,13 @@
     <t>2011/2010/1995/2004/2009/1999</t>
   </si>
   <si>
-    <t>97109/97110/97111/97112/97113/97114</t>
+    <t>0.16/0.07/0.36/0.29/3.58/0.72</t>
   </si>
   <si>
     <t>88/50/68/100/54/125</t>
   </si>
   <si>
-    <t>essence/gazole/gpl/hybride essence/electricite</t>
+    <t>essence/gazole/gpl/hybride essence/NR/electricite</t>
   </si>
   <si>
     <t>300001/300002/300003/300004/300005/300006</t>
@@ -463,15 +481,21 @@
     <t>60/90/120/192/138/95</t>
   </si>
   <si>
+    <t>20226</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>20226</t>
+    <t>28330</t>
   </si>
   <si>
     <t>30000</t>
   </si>
   <si>
+    <t>97110/97111/97112/97113/97114/97115</t>
+  </si>
+  <si>
     <t>O</t>
   </si>
   <si>
@@ -481,7 +505,7 @@
     <t>1957</t>
   </si>
   <si>
-    <t>97110/97111/97112/97113/97114/97115</t>
+    <t>3.58/0.72/1.65/1.35/1.9/2.82</t>
   </si>
   <si>
     <t>170</t>
@@ -967,10 +991,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s" s="19">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E4" t="n" s="21">
         <v>300000.0</v>
@@ -979,13 +1003,13 @@
         <v>0.0</v>
       </c>
       <c r="G4" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H4" t="n" s="24">
         <v>300000.0</v>
       </c>
       <c r="I4" t="s" s="25">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
@@ -993,10 +1017,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s" s="19">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E5" t="n" s="21">
         <v>300000.0</v>
@@ -1005,13 +1029,13 @@
         <v>290.0</v>
       </c>
       <c r="G5" t="s" s="23">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H5" t="n" s="24">
         <v>69.0</v>
       </c>
       <c r="I5" t="s" s="25">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
@@ -1019,10 +1043,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s" s="19">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E6" t="n" s="21">
         <v>300000.0</v>
@@ -1031,13 +1055,13 @@
         <v>290.0</v>
       </c>
       <c r="G6" t="s" s="23">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H6" t="n" s="24">
         <v>70.0</v>
       </c>
       <c r="I6" t="s" s="25">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
@@ -1045,25 +1069,25 @@
         <v>12</v>
       </c>
       <c r="C7" t="s" s="19">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E7" t="n" s="21">
         <v>300000.0</v>
       </c>
       <c r="F7" t="n" s="22">
-        <v>290.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" t="s" s="23">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H7" t="n" s="24">
         <v>155.0</v>
       </c>
       <c r="I7" t="s" s="25">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
@@ -1071,10 +1095,10 @@
         <v>13</v>
       </c>
       <c r="C8" t="s" s="19">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E8" t="n" s="21">
         <v>300000.0</v>
@@ -1083,13 +1107,13 @@
         <v>0.0</v>
       </c>
       <c r="G8" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H8" t="n" s="24">
         <v>51.0</v>
       </c>
       <c r="I8" t="s" s="25">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
@@ -1097,10 +1121,10 @@
         <v>14</v>
       </c>
       <c r="C9" t="s" s="19">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E9" t="n" s="21">
         <v>300000.0</v>
@@ -1109,13 +1133,13 @@
         <v>0.0</v>
       </c>
       <c r="G9" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H9" t="n" s="24">
         <v>44.0</v>
       </c>
       <c r="I9" t="s" s="25">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10">
@@ -1123,25 +1147,25 @@
         <v>15</v>
       </c>
       <c r="C10" t="s" s="19">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E10" t="n" s="21">
         <v>300000.0</v>
       </c>
       <c r="F10" t="n" s="22">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="G10" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H10" t="n" s="24">
         <v>23696.0</v>
       </c>
       <c r="I10" t="s" s="25">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
@@ -1149,25 +1173,25 @@
         <v>16</v>
       </c>
       <c r="C11" t="s" s="19">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E11" t="n" s="21">
         <v>300000.0</v>
       </c>
       <c r="F11" t="n" s="22">
-        <v>413.0</v>
+        <v>0.0</v>
       </c>
       <c r="G11" t="s" s="23">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H11" t="n" s="24">
         <v>6.0</v>
       </c>
       <c r="I11" t="s" s="25">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
@@ -1175,10 +1199,10 @@
         <v>17</v>
       </c>
       <c r="C12" t="s" s="19">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E12" t="n" s="21">
         <v>300000.0</v>
@@ -1187,13 +1211,13 @@
         <v>0.0</v>
       </c>
       <c r="G12" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H12" t="n" s="24">
         <v>1244.0</v>
       </c>
       <c r="I12" t="s" s="25">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13">
@@ -1201,10 +1225,10 @@
         <v>18</v>
       </c>
       <c r="C13" t="s" s="19">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E13" t="n" s="21">
         <v>300000.0</v>
@@ -1213,13 +1237,13 @@
         <v>0.0</v>
       </c>
       <c r="G13" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H13" t="n" s="24">
         <v>149.0</v>
       </c>
       <c r="I13" t="s" s="25">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
@@ -1227,10 +1251,10 @@
         <v>19</v>
       </c>
       <c r="C14" t="s" s="19">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E14" t="n" s="21">
         <v>300000.0</v>
@@ -1239,13 +1263,13 @@
         <v>0.0</v>
       </c>
       <c r="G14" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H14" t="n" s="24">
         <v>17.0</v>
       </c>
       <c r="I14" t="s" s="25">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15">
@@ -1253,10 +1277,10 @@
         <v>20</v>
       </c>
       <c r="C15" t="s" s="19">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E15" t="n" s="21">
         <v>300000.0</v>
@@ -1265,13 +1289,13 @@
         <v>290.0</v>
       </c>
       <c r="G15" t="s" s="23">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H15" t="n" s="24">
         <v>70.0</v>
       </c>
       <c r="I15" t="s" s="25">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16">
@@ -1279,10 +1303,10 @@
         <v>21</v>
       </c>
       <c r="C16" t="s" s="19">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E16" t="n" s="21">
         <v>300000.0</v>
@@ -1291,13 +1315,13 @@
         <v>0.0</v>
       </c>
       <c r="G16" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H16" t="n" s="24">
         <v>6.0</v>
       </c>
       <c r="I16" t="s" s="25">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -1305,10 +1329,10 @@
         <v>22</v>
       </c>
       <c r="C17" t="s" s="19">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E17" t="n" s="21">
         <v>300000.0</v>
@@ -1317,13 +1341,13 @@
         <v>0.0</v>
       </c>
       <c r="G17" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H17" t="n" s="24">
         <v>2.0</v>
       </c>
       <c r="I17" t="s" s="25">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18">
@@ -1331,10 +1355,10 @@
         <v>23</v>
       </c>
       <c r="C18" t="s" s="19">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E18" t="n" s="21">
         <v>300000.0</v>
@@ -1343,13 +1367,13 @@
         <v>0.0</v>
       </c>
       <c r="G18" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H18" t="n" s="24">
         <v>10.0</v>
       </c>
       <c r="I18" t="s" s="25">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19">
@@ -1357,10 +1381,10 @@
         <v>24</v>
       </c>
       <c r="C19" t="s" s="19">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E19" t="n" s="21">
         <v>300000.0</v>
@@ -1369,13 +1393,13 @@
         <v>0.0</v>
       </c>
       <c r="G19" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H19" t="n" s="24">
         <v>2.0</v>
       </c>
       <c r="I19" t="s" s="25">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20">
@@ -1383,10 +1407,10 @@
         <v>25</v>
       </c>
       <c r="C20" t="s" s="19">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E20" t="n" s="21">
         <v>300000.0</v>
@@ -1395,13 +1419,13 @@
         <v>0.0</v>
       </c>
       <c r="G20" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H20" t="n" s="24">
         <v>5.0</v>
       </c>
       <c r="I20" t="s" s="25">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
@@ -1409,25 +1433,25 @@
         <v>26</v>
       </c>
       <c r="C21" t="s" s="19">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E21" t="n" s="21">
         <v>300000.0</v>
       </c>
       <c r="F21" t="n" s="22">
-        <v>290.0</v>
+        <v>0.0</v>
       </c>
       <c r="G21" t="s" s="23">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H21" t="n" s="24">
         <v>19.0</v>
       </c>
       <c r="I21" t="s" s="25">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
@@ -1435,25 +1459,25 @@
         <v>27</v>
       </c>
       <c r="C22" t="s" s="19">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E22" t="n" s="21">
         <v>300000.0</v>
       </c>
       <c r="F22" t="n" s="22">
-        <v>586.0</v>
+        <v>0.0</v>
       </c>
       <c r="G22" t="s" s="23">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H22" t="n" s="24">
         <v>24.0</v>
       </c>
       <c r="I22" t="s" s="25">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23">
@@ -1461,10 +1485,10 @@
         <v>28</v>
       </c>
       <c r="C23" t="s" s="19">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E23" t="n" s="21">
         <v>300000.0</v>
@@ -1473,13 +1497,13 @@
         <v>0.0</v>
       </c>
       <c r="G23" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H23" t="n" s="24">
         <v>335.0</v>
       </c>
       <c r="I23" t="s" s="25">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24">
@@ -1487,10 +1511,10 @@
         <v>29</v>
       </c>
       <c r="C24" t="s" s="19">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E24" t="n" s="21">
         <v>300000.0</v>
@@ -1499,13 +1523,13 @@
         <v>0.0</v>
       </c>
       <c r="G24" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H24" t="n" s="24">
         <v>213.0</v>
       </c>
       <c r="I24" t="s" s="25">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25">
@@ -1513,10 +1537,10 @@
         <v>30</v>
       </c>
       <c r="C25" t="s" s="19">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E25" t="n" s="21">
         <v>300000.0</v>
@@ -1525,13 +1549,13 @@
         <v>0.0</v>
       </c>
       <c r="G25" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H25" t="n" s="24">
         <v>44.0</v>
       </c>
       <c r="I25" t="s" s="25">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26">
@@ -1539,10 +1563,10 @@
         <v>31</v>
       </c>
       <c r="C26" t="s" s="19">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E26" t="n" s="21">
         <v>300000.0</v>
@@ -1551,13 +1575,13 @@
         <v>0.0</v>
       </c>
       <c r="G26" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H26" t="n" s="24">
         <v>1244.0</v>
       </c>
       <c r="I26" t="s" s="25">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
@@ -1565,10 +1589,10 @@
         <v>32</v>
       </c>
       <c r="C27" t="s" s="19">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E27" t="n" s="21">
         <v>300000.0</v>
@@ -1577,13 +1601,13 @@
         <v>0.0</v>
       </c>
       <c r="G27" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H27" t="n" s="24">
         <v>4.0</v>
       </c>
       <c r="I27" t="s" s="25">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28">
@@ -1591,10 +1615,10 @@
         <v>33</v>
       </c>
       <c r="C28" t="s" s="19">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E28" t="n" s="21">
         <v>300000.0</v>
@@ -1603,13 +1627,13 @@
         <v>0.0</v>
       </c>
       <c r="G28" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H28" t="n" s="24">
         <v>8.0</v>
       </c>
       <c r="I28" t="s" s="25">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
@@ -1617,10 +1641,10 @@
         <v>34</v>
       </c>
       <c r="C29" t="s" s="19">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E29" t="n" s="21">
         <v>300000.0</v>
@@ -1629,13 +1653,13 @@
         <v>0.0</v>
       </c>
       <c r="G29" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H29" t="n" s="24">
         <v>10.0</v>
       </c>
       <c r="I29" t="s" s="25">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30">
@@ -1643,25 +1667,25 @@
         <v>35</v>
       </c>
       <c r="C30" t="s" s="19">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D30" t="s" s="20">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E30" t="n" s="21">
         <v>300000.0</v>
       </c>
       <c r="F30" t="n" s="22">
-        <v>329.0</v>
+        <v>0.0</v>
       </c>
       <c r="G30" t="s" s="23">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H30" t="n" s="24">
         <v>7.0</v>
       </c>
       <c r="I30" t="s" s="25">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31">
@@ -1669,10 +1693,10 @@
         <v>36</v>
       </c>
       <c r="C31" t="s" s="19">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E31" t="n" s="21">
         <v>300000.0</v>
@@ -1681,13 +1705,13 @@
         <v>0.0</v>
       </c>
       <c r="G31" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H31" t="n" s="24">
         <v>6.0</v>
       </c>
       <c r="I31" t="s" s="25">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32">
@@ -1695,10 +1719,10 @@
         <v>37</v>
       </c>
       <c r="C32" t="s" s="19">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E32" t="n" s="21">
         <v>300000.0</v>
@@ -1707,13 +1731,13 @@
         <v>0.0</v>
       </c>
       <c r="G32" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H32" t="n" s="24">
         <v>46.0</v>
       </c>
       <c r="I32" t="s" s="25">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33">
@@ -1721,10 +1745,10 @@
         <v>38</v>
       </c>
       <c r="C33" t="s" s="19">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E33" t="n" s="21">
         <v>300000.0</v>
@@ -1733,13 +1757,13 @@
         <v>0.0</v>
       </c>
       <c r="G33" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H33" t="n" s="24">
         <v>29.0</v>
       </c>
       <c r="I33" t="s" s="25">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34">
@@ -1747,10 +1771,10 @@
         <v>39</v>
       </c>
       <c r="C34" t="s" s="19">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E34" t="n" s="21">
         <v>300000.0</v>
@@ -1759,13 +1783,13 @@
         <v>0.0</v>
       </c>
       <c r="G34" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H34" t="n" s="24">
         <v>2.0</v>
       </c>
       <c r="I34" t="s" s="25">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35">
@@ -1773,10 +1797,10 @@
         <v>40</v>
       </c>
       <c r="C35" t="s" s="19">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E35" t="n" s="21">
         <v>300000.0</v>
@@ -1785,13 +1809,13 @@
         <v>0.0</v>
       </c>
       <c r="G35" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H35" t="n" s="24">
         <v>2.0</v>
       </c>
       <c r="I35" t="s" s="25">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36">
@@ -1799,10 +1823,10 @@
         <v>41</v>
       </c>
       <c r="C36" t="s" s="19">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s" s="20">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E36" t="n" s="21">
         <v>300000.0</v>
@@ -1811,13 +1835,13 @@
         <v>0.0</v>
       </c>
       <c r="G36" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H36" t="n" s="24">
         <v>25.0</v>
       </c>
       <c r="I36" t="s" s="25">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37">
@@ -1825,10 +1849,10 @@
         <v>42</v>
       </c>
       <c r="C37" t="s" s="19">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D37" t="s" s="20">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E37" t="n" s="21">
         <v>300000.0</v>
@@ -1837,13 +1861,91 @@
         <v>0.0</v>
       </c>
       <c r="G37" t="s" s="23">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H37" t="n" s="24">
         <v>52717.0</v>
       </c>
       <c r="I37" t="s" s="25">
-        <v>116</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s" s="14">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s" s="19">
+        <v>80</v>
+      </c>
+      <c r="D38" t="s" s="20">
+        <v>85</v>
+      </c>
+      <c r="E38" t="n" s="21">
+        <v>300000.0</v>
+      </c>
+      <c r="F38" t="n" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="G38" t="s" s="23">
+        <v>86</v>
+      </c>
+      <c r="H38" t="n" s="24">
+        <v>174228.0</v>
+      </c>
+      <c r="I38" t="s" s="25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s" s="14">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s" s="19">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s" s="20">
+        <v>84</v>
+      </c>
+      <c r="E39" t="n" s="21">
+        <v>300000.0</v>
+      </c>
+      <c r="F39" t="n" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="G39" t="s" s="23">
+        <v>86</v>
+      </c>
+      <c r="H39" t="n" s="24">
+        <v>23696.0</v>
+      </c>
+      <c r="I39" t="s" s="25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s" s="19">
+        <v>82</v>
+      </c>
+      <c r="D40" t="s" s="20">
+        <v>85</v>
+      </c>
+      <c r="E40" t="n" s="21">
+        <v>300000.0</v>
+      </c>
+      <c r="F40" t="n" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="G40" t="s" s="23">
+        <v>86</v>
+      </c>
+      <c r="H40" t="n" s="24">
+        <v>47.0</v>
+      </c>
+      <c r="I40" t="s" s="25">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1874,7 +1976,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="s" s="27">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
@@ -1906,10 +2008,10 @@
         <v>8</v>
       </c>
       <c r="J3" t="s" s="43">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="K3" t="s" s="43">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4">
@@ -1917,10 +2019,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s" s="44">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E4" t="n" s="46">
         <v>30000.0</v>
@@ -1929,19 +2031,19 @@
         <v>0.0</v>
       </c>
       <c r="G4" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H4" t="n" s="49">
-        <v>44.0</v>
+        <v>50.0</v>
       </c>
       <c r="I4" t="s" s="50">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="J4" t="s" s="51">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="K4" t="s" s="52">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5">
@@ -1949,31 +2051,31 @@
         <v>10</v>
       </c>
       <c r="C5" t="s" s="44">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E5" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F5" t="n" s="47">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="G5" t="s" s="48">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="H5" t="n" s="49">
-        <v>51.0</v>
+        <v>44.0</v>
       </c>
       <c r="I5" t="s" s="50">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="J5" t="s" s="51">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="K5" t="s" s="52">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6">
@@ -1981,10 +2083,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s" s="44">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E6" t="n" s="46">
         <v>30000.0</v>
@@ -1993,19 +2095,19 @@
         <v>17.0</v>
       </c>
       <c r="G6" t="s" s="48">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="H6" t="n" s="49">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="I6" t="s" s="50">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="J6" t="s" s="51">
         <v>9</v>
       </c>
       <c r="K6" t="s" s="52">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7">
@@ -2013,31 +2115,31 @@
         <v>12</v>
       </c>
       <c r="C7" t="s" s="44">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E7" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F7" t="n" s="47">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
       <c r="G7" t="s" s="48">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="H7" t="n" s="49">
-        <v>50.0</v>
+        <v>52.0</v>
       </c>
       <c r="I7" t="s" s="50">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="J7" t="s" s="51">
-        <v>150</v>
+        <v>9</v>
       </c>
       <c r="K7" t="s" s="52">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8">
@@ -2048,7 +2150,7 @@
         <v>52</v>
       </c>
       <c r="D8" t="s" s="45">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E8" t="n" s="46">
         <v>30000.0</v>
@@ -2057,19 +2159,19 @@
         <v>0.0</v>
       </c>
       <c r="G8" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H8" t="n" s="49">
-        <v>104.0</v>
+        <v>50.0</v>
       </c>
       <c r="I8" t="s" s="50">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J8" t="s" s="51">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="K8" t="s" s="52">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9">
@@ -2077,31 +2179,31 @@
         <v>14</v>
       </c>
       <c r="C9" t="s" s="44">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s" s="45">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E9" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F9" t="n" s="47">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="G9" t="s" s="48">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="H9" t="n" s="49">
-        <v>6.0</v>
+        <v>44.0</v>
       </c>
       <c r="I9" t="s" s="50">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="J9" t="s" s="51">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="K9" t="s" s="52">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10">
@@ -2109,10 +2211,10 @@
         <v>15</v>
       </c>
       <c r="C10" t="s" s="44">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E10" t="n" s="46">
         <v>30000.0</v>
@@ -2121,19 +2223,19 @@
         <v>0.0</v>
       </c>
       <c r="G10" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H10" t="n" s="49">
-        <v>30000.0</v>
+        <v>104.0</v>
       </c>
       <c r="I10" t="s" s="50">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="J10" t="s" s="51">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="K10" t="s" s="52">
-        <v>127</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11">
@@ -2141,10 +2243,10 @@
         <v>16</v>
       </c>
       <c r="C11" t="s" s="44">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s" s="45">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E11" t="n" s="46">
         <v>30000.0</v>
@@ -2153,19 +2255,19 @@
         <v>0.0</v>
       </c>
       <c r="G11" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H11" t="n" s="49">
-        <v>900.0</v>
+        <v>6.0</v>
       </c>
       <c r="I11" t="s" s="50">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="J11" t="s" s="51">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="K11" t="s" s="52">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12">
@@ -2176,28 +2278,28 @@
         <v>46</v>
       </c>
       <c r="D12" t="s" s="45">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E12" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F12" t="n" s="47">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="G12" t="s" s="48">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="H12" t="n" s="49">
-        <v>74.0</v>
+        <v>30000.0</v>
       </c>
       <c r="I12" t="s" s="50">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="J12" t="s" s="51">
-        <v>10</v>
+        <v>158</v>
       </c>
       <c r="K12" t="s" s="52">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13">
@@ -2205,10 +2307,10 @@
         <v>18</v>
       </c>
       <c r="C13" t="s" s="44">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s" s="45">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E13" t="n" s="46">
         <v>30000.0</v>
@@ -2217,19 +2319,19 @@
         <v>0.0</v>
       </c>
       <c r="G13" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H13" t="n" s="49">
-        <v>17.0</v>
+        <v>900.0</v>
       </c>
       <c r="I13" t="s" s="50">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="J13" t="s" s="51">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s" s="52">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14">
@@ -2237,10 +2339,10 @@
         <v>19</v>
       </c>
       <c r="C14" t="s" s="44">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s" s="45">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E14" t="n" s="46">
         <v>30000.0</v>
@@ -2249,19 +2351,19 @@
         <v>0.0</v>
       </c>
       <c r="G14" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H14" t="n" s="49">
-        <v>36.0</v>
+        <v>74.0</v>
       </c>
       <c r="I14" t="s" s="50">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="J14" t="s" s="51">
-        <v>149</v>
+        <v>10</v>
       </c>
       <c r="K14" t="s" s="52">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
@@ -2269,31 +2371,31 @@
         <v>20</v>
       </c>
       <c r="C15" t="s" s="44">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s" s="45">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E15" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F15" t="n" s="47">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="s" s="48">
+        <v>86</v>
+      </c>
+      <c r="H15" t="n" s="49">
         <v>17.0</v>
       </c>
-      <c r="G15" t="s" s="48">
-        <v>120</v>
-      </c>
-      <c r="H15" t="n" s="49">
-        <v>52.0</v>
-      </c>
       <c r="I15" t="s" s="50">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="J15" t="s" s="51">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="K15" t="s" s="52">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16">
@@ -2301,10 +2403,10 @@
         <v>21</v>
       </c>
       <c r="C16" t="s" s="44">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E16" t="n" s="46">
         <v>30000.0</v>
@@ -2313,19 +2415,19 @@
         <v>0.0</v>
       </c>
       <c r="G16" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H16" t="n" s="49">
-        <v>160.0</v>
+        <v>36.0</v>
       </c>
       <c r="I16" t="s" s="50">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="J16" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K16" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17">
@@ -2333,31 +2435,31 @@
         <v>22</v>
       </c>
       <c r="C17" t="s" s="44">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E17" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F17" t="n" s="47">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
       <c r="G17" t="s" s="48">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="H17" t="n" s="49">
-        <v>44.0</v>
+        <v>52.0</v>
       </c>
       <c r="I17" t="s" s="50">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="J17" t="s" s="51">
-        <v>149</v>
+        <v>9</v>
       </c>
       <c r="K17" t="s" s="52">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18">
@@ -2365,10 +2467,10 @@
         <v>23</v>
       </c>
       <c r="C18" t="s" s="44">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E18" t="n" s="46">
         <v>30000.0</v>
@@ -2377,16 +2479,16 @@
         <v>0.0</v>
       </c>
       <c r="G18" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H18" t="n" s="49">
-        <v>899.0</v>
+        <v>160.0</v>
       </c>
       <c r="I18" t="s" s="50">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="J18" t="s" s="51">
-        <v>33</v>
+        <v>156</v>
       </c>
       <c r="K18" t="s" s="52">
         <v>160</v>
@@ -2397,10 +2499,10 @@
         <v>24</v>
       </c>
       <c r="C19" t="s" s="44">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E19" t="n" s="46">
         <v>30000.0</v>
@@ -2409,19 +2511,19 @@
         <v>0.0</v>
       </c>
       <c r="G19" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H19" t="n" s="49">
-        <v>4.0</v>
+        <v>44.0</v>
       </c>
       <c r="I19" t="s" s="50">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="J19" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K19" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20">
@@ -2429,10 +2531,10 @@
         <v>25</v>
       </c>
       <c r="C20" t="s" s="44">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s" s="45">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E20" t="n" s="46">
         <v>30000.0</v>
@@ -2441,19 +2543,19 @@
         <v>0.0</v>
       </c>
       <c r="G20" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H20" t="n" s="49">
-        <v>1.0</v>
+        <v>899.0</v>
       </c>
       <c r="I20" t="s" s="50">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J20" t="s" s="51">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="K20" t="s" s="52">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21">
@@ -2461,10 +2563,10 @@
         <v>26</v>
       </c>
       <c r="C21" t="s" s="44">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E21" t="n" s="46">
         <v>30000.0</v>
@@ -2473,19 +2575,19 @@
         <v>0.0</v>
       </c>
       <c r="G21" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H21" t="n" s="49">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="I21" t="s" s="50">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="J21" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K21" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22">
@@ -2493,31 +2595,31 @@
         <v>27</v>
       </c>
       <c r="C22" t="s" s="44">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s" s="45">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E22" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F22" t="n" s="47">
-        <v>41.0</v>
+        <v>0.0</v>
       </c>
       <c r="G22" t="s" s="48">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H22" t="n" s="49">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="I22" t="s" s="50">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="J22" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K22" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23">
@@ -2525,10 +2627,10 @@
         <v>28</v>
       </c>
       <c r="C23" t="s" s="44">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E23" t="n" s="46">
         <v>30000.0</v>
@@ -2537,19 +2639,19 @@
         <v>0.0</v>
       </c>
       <c r="G23" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H23" t="n" s="49">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="I23" t="s" s="50">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="J23" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K23" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24">
@@ -2557,10 +2659,10 @@
         <v>29</v>
       </c>
       <c r="C24" t="s" s="44">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s" s="45">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E24" t="n" s="46">
         <v>30000.0</v>
@@ -2569,19 +2671,19 @@
         <v>0.0</v>
       </c>
       <c r="G24" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H24" t="n" s="49">
-        <v>23.0</v>
+        <v>7.0</v>
       </c>
       <c r="I24" t="s" s="50">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="J24" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K24" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25">
@@ -2589,10 +2691,10 @@
         <v>30</v>
       </c>
       <c r="C25" t="s" s="44">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E25" t="n" s="46">
         <v>30000.0</v>
@@ -2601,19 +2703,19 @@
         <v>0.0</v>
       </c>
       <c r="G25" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H25" t="n" s="49">
-        <v>16.0</v>
+        <v>6.0</v>
       </c>
       <c r="I25" t="s" s="50">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="J25" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K25" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26">
@@ -2621,10 +2723,10 @@
         <v>31</v>
       </c>
       <c r="C26" t="s" s="44">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E26" t="n" s="46">
         <v>30000.0</v>
@@ -2633,19 +2735,19 @@
         <v>0.0</v>
       </c>
       <c r="G26" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H26" t="n" s="49">
-        <v>6.0</v>
+        <v>23.0</v>
       </c>
       <c r="I26" t="s" s="50">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="J26" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K26" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27">
@@ -2653,10 +2755,10 @@
         <v>32</v>
       </c>
       <c r="C27" t="s" s="44">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E27" t="n" s="46">
         <v>30000.0</v>
@@ -2665,19 +2767,19 @@
         <v>0.0</v>
       </c>
       <c r="G27" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H27" t="n" s="49">
-        <v>2.0</v>
+        <v>16.0</v>
       </c>
       <c r="I27" t="s" s="50">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="J27" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K27" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28">
@@ -2685,10 +2787,10 @@
         <v>33</v>
       </c>
       <c r="C28" t="s" s="44">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E28" t="n" s="46">
         <v>30000.0</v>
@@ -2697,19 +2799,19 @@
         <v>0.0</v>
       </c>
       <c r="G28" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H28" t="n" s="49">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="I28" t="s" s="50">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="J28" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K28" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29">
@@ -2717,10 +2819,10 @@
         <v>34</v>
       </c>
       <c r="C29" t="s" s="44">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E29" t="n" s="46">
         <v>30000.0</v>
@@ -2729,19 +2831,19 @@
         <v>0.0</v>
       </c>
       <c r="G29" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H29" t="n" s="49">
-        <v>13.0</v>
+        <v>2.0</v>
       </c>
       <c r="I29" t="s" s="50">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="J29" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K29" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30">
@@ -2749,10 +2851,10 @@
         <v>35</v>
       </c>
       <c r="C30" t="s" s="44">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E30" t="n" s="46">
         <v>30000.0</v>
@@ -2761,19 +2863,19 @@
         <v>0.0</v>
       </c>
       <c r="G30" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H30" t="n" s="49">
         <v>2.0</v>
       </c>
       <c r="I30" t="s" s="50">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="J30" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K30" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31">
@@ -2781,10 +2883,10 @@
         <v>36</v>
       </c>
       <c r="C31" t="s" s="44">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E31" t="n" s="46">
         <v>30000.0</v>
@@ -2793,19 +2895,19 @@
         <v>0.0</v>
       </c>
       <c r="G31" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H31" t="n" s="49">
-        <v>10.0</v>
+        <v>13.0</v>
       </c>
       <c r="I31" t="s" s="50">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="J31" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K31" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32">
@@ -2813,10 +2915,10 @@
         <v>37</v>
       </c>
       <c r="C32" t="s" s="44">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s" s="45">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E32" t="n" s="46">
         <v>30000.0</v>
@@ -2825,19 +2927,19 @@
         <v>0.0</v>
       </c>
       <c r="G32" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H32" t="n" s="49">
         <v>2.0</v>
       </c>
       <c r="I32" t="s" s="50">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J32" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K32" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33">
@@ -2845,10 +2947,10 @@
         <v>38</v>
       </c>
       <c r="C33" t="s" s="44">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s" s="45">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E33" t="n" s="46">
         <v>30000.0</v>
@@ -2857,19 +2959,19 @@
         <v>0.0</v>
       </c>
       <c r="G33" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H33" t="n" s="49">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="I33" t="s" s="50">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="J33" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K33" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34">
@@ -2877,31 +2979,31 @@
         <v>39</v>
       </c>
       <c r="C34" t="s" s="44">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s" s="45">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E34" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F34" t="n" s="47">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="G34" t="s" s="48">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="H34" t="n" s="49">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
       <c r="I34" t="s" s="50">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="J34" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K34" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35">
@@ -2909,31 +3011,31 @@
         <v>40</v>
       </c>
       <c r="C35" t="s" s="44">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s" s="45">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E35" t="n" s="46">
         <v>30000.0</v>
       </c>
       <c r="F35" t="n" s="47">
-        <v>18.0</v>
+        <v>0.0</v>
       </c>
       <c r="G35" t="s" s="48">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="H35" t="n" s="49">
-        <v>20.0</v>
+        <v>5.0</v>
       </c>
       <c r="I35" t="s" s="50">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="J35" t="s" s="51">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K35" t="s" s="52">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36">
@@ -2941,10 +3043,10 @@
         <v>41</v>
       </c>
       <c r="C36" t="s" s="44">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s" s="45">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E36" t="n" s="46">
         <v>30000.0</v>
@@ -2953,19 +3055,83 @@
         <v>0.0</v>
       </c>
       <c r="G36" t="s" s="48">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H36" t="n" s="49">
+        <v>17.0</v>
+      </c>
+      <c r="I36" t="s" s="50">
+        <v>152</v>
+      </c>
+      <c r="J36" t="s" s="51">
+        <v>156</v>
+      </c>
+      <c r="K36" t="s" s="52">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s" s="39">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s" s="44">
+        <v>64</v>
+      </c>
+      <c r="D37" t="s" s="45">
+        <v>84</v>
+      </c>
+      <c r="E37" t="n" s="46">
+        <v>30000.0</v>
+      </c>
+      <c r="F37" t="n" s="47">
+        <v>0.0</v>
+      </c>
+      <c r="G37" t="s" s="48">
+        <v>86</v>
+      </c>
+      <c r="H37" t="n" s="49">
+        <v>20.0</v>
+      </c>
+      <c r="I37" t="s" s="50">
+        <v>153</v>
+      </c>
+      <c r="J37" t="s" s="51">
+        <v>156</v>
+      </c>
+      <c r="K37" t="s" s="52">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s" s="39">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s" s="44">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s" s="45">
+        <v>83</v>
+      </c>
+      <c r="E38" t="n" s="46">
+        <v>30000.0</v>
+      </c>
+      <c r="F38" t="n" s="47">
+        <v>0.0</v>
+      </c>
+      <c r="G38" t="s" s="48">
+        <v>86</v>
+      </c>
+      <c r="H38" t="n" s="49">
         <v>221.0</v>
       </c>
-      <c r="I36" t="s" s="50">
-        <v>148</v>
-      </c>
-      <c r="J36" t="s" s="51">
-        <v>149</v>
-      </c>
-      <c r="K36" t="s" s="52">
-        <v>152</v>
+      <c r="I38" t="s" s="50">
+        <v>154</v>
+      </c>
+      <c r="J38" t="s" s="51">
+        <v>156</v>
+      </c>
+      <c r="K38" t="s" s="52">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2989,7 +3155,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="s" s="54">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2">
@@ -3000,10 +3166,10 @@
     <row r="3">
       <c r="B3"/>
       <c r="C3" t="s" s="70">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s" s="70">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4">
@@ -3011,10 +3177,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s" s="71">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D4" t="n" s="72">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="5">
@@ -3022,7 +3188,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s" s="71">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D5" t="n" s="72">
         <v>24.0</v>
@@ -3033,10 +3199,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s" s="71">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D6" t="n" s="72">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>